<commit_message>
updated test case and utility file
</commit_message>
<xml_diff>
--- a/vtigerCRM/src/main/resources/vtiger Test Cases.xlsx
+++ b/vtigerCRM/src/main/resources/vtiger Test Cases.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisha\git\repository6\vtigerCRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266EE95C-5363-4354-8A5D-64AB46F739D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413779D1-3838-4BA3-8C7D-5FA23D83C2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00E9E43E-9B59-4541-A21B-383CAFE760CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="System and smoke " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>ProjectName</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>vtigerCRM</t>
+  </si>
+  <si>
+    <t>*URL:http://localhost:8888/
+*User Name: admin                                                                                        *Password: root                                                                                     *lasrtName : Amazon
+industry: anyone(from the dropdown)
+typeDropDown : (anyone)</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -566,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -578,9 +584,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -605,7 +608,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F576F174-B356-44D8-A03C-516874ACD94F}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="54" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,39 +978,39 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="119.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1016,7 +1019,7 @@
       <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -1025,7 +1028,7 @@
       <c r="F6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -1035,7 +1038,7 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="119.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1044,7 +1047,7 @@
       <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="9" t="s">
@@ -1053,8 +1056,8 @@
       <c r="F7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>24</v>
+      <c r="G7" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>25</v>
@@ -1063,7 +1066,7 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1072,7 +1075,7 @@
       <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1091,16 +1094,16 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -1109,7 +1112,7 @@
       <c r="F9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -1119,18 +1122,18 @@
       <c r="J9" s="4"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified utilities files, added testscripts and generated test scripts based on the testcases and requirement and prepared extent report and took screenshot for failed testscript.
</commit_message>
<xml_diff>
--- a/vtigerCRM/src/main/resources/vtiger Test Cases.xlsx
+++ b/vtigerCRM/src/main/resources/vtiger Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisha\git\repository6\vtigerCRM\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413779D1-3838-4BA3-8C7D-5FA23D83C2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F44D5C-5030-4628-8CCF-4EA5A7AA132B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00E9E43E-9B59-4541-A21B-383CAFE760CF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>ProjectName</t>
   </si>
@@ -277,6 +277,24 @@
 3. Enter text in "username" text filed
 4. Enter text in "Password" text field     
 5. Click on "Login" button                                                                                                                                                                                                                                                                                                                                                                 6. Navigate to Contacts link                                                                                                                                                                                                                                                                                                                                                                  7. Click on Create Contact                                                                                                                            8. Select Prefix                                                                                                                                                                                                                                                                                                                                                                          9. Enter First Name                                                                                                                                              10. Enter Last Name                                                                                                                                                                           11. Select Organization Name                                                                                                                           12. Select Lead Source                                                                                                                           13. Select Lead Source                                                                                                                                                          14. Enter Title                                                                                                                                                                   15. Enter Department                                                                                                                                                      16. Enter Email                                                                                                                                                                  17. Enter Assistant                                                                                                                                 18. Enter Assistant phone                                                                                                                                  19. Check all Check Box                                                                                                                                                                   20. Enter Office Phone                                                                                                                                                                            21. Enter Mobile                                                                                                                                                          22. Enter Home Phone                                                                                                                                                   23. Enter Other Phone                                                                                                                     24. Enter Fax                                                                                                                                                 25. Enter BirthDate                                                                                                                                           26. Select Report to                                                                                                                                        27. Enter Secondary Email                                                                                                                                     28. Click On Save button and Verify the contact                                                                                 29. Logout                                                                                                                                                                        30. Close the Browser</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Approved By</t>
+  </si>
+  <si>
+    <t>Approved Date</t>
+  </si>
+  <si>
+    <t>vtigerCRM</t>
+  </si>
+  <si>
+    <t>*URL:http://localhost:8888/
+*User Name: admin                                                                                        *Password: root                                                                                     *lasrtName : Amazon
+industry: anyone(from the dropdown)
+typeDropDown : (anyone)</t>
   </si>
   <si>
     <t>*URL:http://localhost:8888/
@@ -288,7 +306,7 @@
 Hero
 Super Heros
 shinchan@gmail.com
-Geeta Vishwas
+Narendra Modi
 9999999999
 8888888888
 7777777777
@@ -300,22 +318,52 @@
 Not Applicable</t>
   </si>
   <si>
-    <t>Reviewed By</t>
-  </si>
-  <si>
-    <t>Approved By</t>
-  </si>
-  <si>
-    <t>Approved Date</t>
-  </si>
-  <si>
-    <t>vtigerCRM</t>
-  </si>
-  <si>
-    <t>*URL:http://localhost:8888/
-*User Name: admin                                                                                        *Password: root                                                                                     *lasrtName : Amazon
-industry: anyone(from the dropdown)
-typeDropDown : (anyone)</t>
+    <r>
+      <t>*Homepage should be displayed.          
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Creating New Organization </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page should display.                                 *</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Organization Information </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>page should be displayed.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -935,7 +983,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
@@ -1032,7 +1080,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1057,7 +1105,7 @@
         <v>29</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>25</v>
@@ -1113,7 +1161,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>33</v>
@@ -1123,18 +1171,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>